<commit_message>
Added row to project list
</commit_message>
<xml_diff>
--- a/Operations/ATA_Operations.xlsx
+++ b/Operations/ATA_Operations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Targeted RFI Assessment</t>
+  </si>
+  <si>
+    <t>SETI Planet-Planet Occultation Search</t>
+  </si>
+  <si>
+    <t>In collaboration with folks at the PSETI Center</t>
   </si>
   <si>
     <t>???</t>
@@ -2138,7 +2144,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F14"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2309,25 +2315,27 @@
       </c>
       <c r="F9" s="34"/>
     </row>
-    <row r="10" ht="25.35" customHeight="1">
-      <c r="A10" t="s" s="32">
+    <row r="10" ht="32.05" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" t="s" s="17">
         <v>74</v>
       </c>
-      <c r="B10" t="s" s="17">
-        <v>75</v>
-      </c>
       <c r="C10" t="s" s="14">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s" s="31">
         <v>57</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" ht="32.05" customHeight="1">
+      <c r="E10" t="s" s="15">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s" s="15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" ht="25.35" customHeight="1">
       <c r="A11" t="s" s="32">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s" s="17">
         <v>77</v>
@@ -2341,15 +2349,15 @@
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
     </row>
-    <row r="12" ht="25.35" customHeight="1">
+    <row r="12" ht="32.05" customHeight="1">
       <c r="A12" t="s" s="32">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s" s="17">
         <v>79</v>
       </c>
       <c r="C12" t="s" s="14">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s" s="31">
         <v>57</v>
@@ -2357,15 +2365,15 @@
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
     </row>
-    <row r="13" ht="32.05" customHeight="1">
+    <row r="13" ht="25.35" customHeight="1">
       <c r="A13" t="s" s="32">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s" s="17">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s" s="14">
         <v>80</v>
-      </c>
-      <c r="C13" t="s" s="14">
-        <v>78</v>
       </c>
       <c r="D13" t="s" s="31">
         <v>57</v>
@@ -2375,25 +2383,41 @@
     </row>
     <row r="14" ht="32.05" customHeight="1">
       <c r="A14" t="s" s="32">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s" s="17">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s" s="14">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s" s="31">
         <v>57</v>
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
+    </row>
+    <row r="15" ht="32.05" customHeight="1">
+      <c r="A15" t="s" s="32">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s" s="17">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s" s="14">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s" s="31">
+        <v>57</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A6:A10"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>